<commit_message>
excluded SOH from cosponsor analysis
</commit_message>
<xml_diff>
--- a/output/working_joined_hr1296.xlsx
+++ b/output/working_joined_hr1296.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BM236"/>
+  <dimension ref="A1:BM235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -52614,7 +52614,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -52868,7 +52868,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -53122,7 +53122,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -53620,7 +53620,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -53875,7 +53875,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -54135,7 +54135,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -54395,7 +54395,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -54649,7 +54649,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -54909,7 +54909,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -55163,7 +55163,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -55412,7 +55412,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -55667,7 +55667,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -55927,7 +55927,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -56182,7 +56182,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -56382,7 +56382,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -56636,7 +56636,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -56890,7 +56890,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -56900,17 +56900,22 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>P000197</t>
+          <t>P000258</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Nancy</t>
+          <t>Collin</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>C.</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>Pelosi</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -56920,22 +56925,22 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>0612</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>H8CA05035</t>
+          <t>H2MN07014</t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
@@ -56949,10 +56954,10 @@
         </is>
       </c>
       <c r="N227">
-        <v>86.8</v>
+        <v>52.1</v>
       </c>
       <c r="O227">
-        <v>13.2</v>
+        <v>47.9</v>
       </c>
       <c r="P227" t="inlineStr">
         <is>
@@ -56960,38 +56965,38 @@
         </is>
       </c>
       <c r="Q227">
-        <v>73.59999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="R227" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="S227" t="inlineStr">
         <is>
-          <t>CA-12</t>
+          <t>MN-07</t>
         </is>
       </c>
       <c r="U227">
-        <v>740337</v>
+        <v>663338</v>
       </c>
       <c r="V227">
-        <v>88364</v>
+        <v>52930</v>
       </c>
       <c r="W227">
-        <v>38.2</v>
+        <v>40.7</v>
       </c>
       <c r="X227">
-        <v>33.735</v>
+        <v>2.978</v>
       </c>
       <c r="Y227">
-        <v>3.516</v>
+        <v>9.205</v>
       </c>
       <c r="Z227">
-        <v>56.535</v>
+        <v>10.608</v>
       </c>
       <c r="AA227">
-        <v>56.325</v>
+        <v>21.486</v>
       </c>
       <c r="AB227">
         <v>55322</v>
@@ -57013,7 +57018,7 @@
       </c>
       <c r="AH227" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AI227" t="inlineStr">
@@ -57023,53 +57028,53 @@
       </c>
       <c r="AJ227" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AK227" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AL227" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AM227" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AN227">
-        <v>80.90000000000001</v>
+        <v>52.5</v>
       </c>
       <c r="AO227">
-        <v>0</v>
+        <v>47.4</v>
       </c>
       <c r="AP227">
-        <v>85.2</v>
+        <v>30.8</v>
       </c>
       <c r="AQ227">
-        <v>8.6</v>
+        <v>61.4</v>
       </c>
       <c r="AR227">
-        <v>83.3</v>
+        <v>54.3</v>
       </c>
       <c r="AS227">
-        <v>16.7</v>
+        <v>45.7</v>
       </c>
       <c r="AT227">
-        <v>85.09999999999999</v>
+        <v>60.4</v>
       </c>
       <c r="AU227">
-        <v>14.9</v>
+        <v>34.8</v>
       </c>
       <c r="AV227">
-        <v>84.09999999999999</v>
+        <v>44</v>
       </c>
       <c r="AW227">
-        <v>12.5</v>
+        <v>53.7</v>
       </c>
       <c r="AX227" t="inlineStr">
         <is>
@@ -57078,7 +57083,7 @@
       </c>
       <c r="AY227" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AZ227" t="inlineStr">
@@ -57093,7 +57098,7 @@
       </c>
       <c r="BB227" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BC227" t="inlineStr">
@@ -57102,32 +57107,32 @@
         </is>
       </c>
       <c r="BD227">
-        <v>0</v>
+        <v>64.13</v>
       </c>
       <c r="BE227" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BF227" t="inlineStr">
         <is>
-          <t>below 20th percentile</t>
+          <t>80th percentile and above</t>
         </is>
       </c>
       <c r="BG227" t="inlineStr">
         <is>
-          <t>$121,110.56</t>
+          <t>$25,434.69</t>
         </is>
       </c>
       <c r="BH227">
-        <v>121110.56</v>
+        <v>25434.69</v>
       </c>
       <c r="BI227">
         <v>38182.45</v>
       </c>
       <c r="BJ227" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BK227" t="inlineStr">
@@ -57139,7 +57144,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -57149,22 +57154,17 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>P000258</t>
+          <t>S001180</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Collin</t>
-        </is>
-      </c>
-      <c r="E228" t="inlineStr">
-        <is>
-          <t>C.</t>
+          <t>Kurt</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Schrader</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -57174,22 +57174,22 @@
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>4105</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t>H2MN07014</t>
+          <t>H8OR05107</t>
         </is>
       </c>
       <c r="L228" t="inlineStr">
@@ -57203,10 +57203,10 @@
         </is>
       </c>
       <c r="N228">
-        <v>52.1</v>
+        <v>55.1</v>
       </c>
       <c r="O228">
-        <v>47.9</v>
+        <v>41.9</v>
       </c>
       <c r="P228" t="inlineStr">
         <is>
@@ -57214,38 +57214,38 @@
         </is>
       </c>
       <c r="Q228">
-        <v>4.2</v>
+        <v>13.2</v>
       </c>
       <c r="R228" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="S228" t="inlineStr">
         <is>
-          <t>MN-07</t>
+          <t>OR-05</t>
         </is>
       </c>
       <c r="U228">
-        <v>663338</v>
+        <v>795885</v>
       </c>
       <c r="V228">
-        <v>52930</v>
+        <v>56481</v>
       </c>
       <c r="W228">
-        <v>40.7</v>
+        <v>39.2</v>
       </c>
       <c r="X228">
-        <v>2.978</v>
+        <v>9.961</v>
       </c>
       <c r="Y228">
-        <v>9.205</v>
+        <v>9.831</v>
       </c>
       <c r="Z228">
-        <v>10.608</v>
+        <v>24.077</v>
       </c>
       <c r="AA228">
-        <v>21.486</v>
+        <v>29.316</v>
       </c>
       <c r="AB228">
         <v>55322</v>
@@ -57267,7 +57267,7 @@
       </c>
       <c r="AH228" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AI228" t="inlineStr">
@@ -57296,34 +57296,34 @@
         </is>
       </c>
       <c r="AN228">
-        <v>52.5</v>
+        <v>53.5</v>
       </c>
       <c r="AO228">
-        <v>47.4</v>
+        <v>43</v>
       </c>
       <c r="AP228">
-        <v>30.8</v>
+        <v>46.4</v>
       </c>
       <c r="AQ228">
-        <v>61.4</v>
+        <v>42.3</v>
       </c>
       <c r="AR228">
-        <v>54.3</v>
+        <v>53.8</v>
       </c>
       <c r="AS228">
-        <v>45.7</v>
+        <v>39.4</v>
       </c>
       <c r="AT228">
-        <v>60.4</v>
+        <v>54</v>
       </c>
       <c r="AU228">
-        <v>34.8</v>
+        <v>42.4</v>
       </c>
       <c r="AV228">
-        <v>44</v>
+        <v>50.1</v>
       </c>
       <c r="AW228">
-        <v>53.7</v>
+        <v>46.8</v>
       </c>
       <c r="AX228" t="inlineStr">
         <is>
@@ -57332,7 +57332,7 @@
       </c>
       <c r="AY228" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AZ228" t="inlineStr">
@@ -57347,7 +57347,7 @@
       </c>
       <c r="BB228" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BC228" t="inlineStr">
@@ -57356,25 +57356,25 @@
         </is>
       </c>
       <c r="BD228">
-        <v>64.13</v>
+        <v>15.74</v>
       </c>
       <c r="BE228" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BF228" t="inlineStr">
         <is>
-          <t>80th percentile and above</t>
+          <t>40th percentile</t>
         </is>
       </c>
       <c r="BG228" t="inlineStr">
         <is>
-          <t>$25,434.69</t>
+          <t>$33,224.25</t>
         </is>
       </c>
       <c r="BH228">
-        <v>25434.69</v>
+        <v>33224.25</v>
       </c>
       <c r="BI228">
         <v>38182.45</v>
@@ -57393,7 +57393,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -57403,17 +57403,17 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>S001180</t>
+          <t>S001185</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Kurt</t>
+          <t>Terri</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Schrader</t>
+          <t>Sewell</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
@@ -57423,22 +57423,22 @@
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>4105</t>
+          <t>0107</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>H8OR05107</t>
+          <t>H0AL07086</t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
@@ -57452,10 +57452,10 @@
         </is>
       </c>
       <c r="N229">
-        <v>55.1</v>
+        <v>100</v>
       </c>
       <c r="O229">
-        <v>41.9</v>
+        <v>0</v>
       </c>
       <c r="P229" t="inlineStr">
         <is>
@@ -57463,38 +57463,38 @@
         </is>
       </c>
       <c r="Q229">
-        <v>13.2</v>
+        <v>100</v>
       </c>
       <c r="R229" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="S229" t="inlineStr">
         <is>
-          <t>OR-05</t>
+          <t>AL-07</t>
         </is>
       </c>
       <c r="U229">
-        <v>795885</v>
+        <v>675230</v>
       </c>
       <c r="V229">
-        <v>56481</v>
+        <v>33366</v>
       </c>
       <c r="W229">
-        <v>39.2</v>
+        <v>35.8</v>
       </c>
       <c r="X229">
-        <v>9.961</v>
+        <v>2.556</v>
       </c>
       <c r="Y229">
-        <v>9.831</v>
+        <v>7.464</v>
       </c>
       <c r="Z229">
-        <v>24.077</v>
+        <v>67.965</v>
       </c>
       <c r="AA229">
-        <v>29.316</v>
+        <v>19.1</v>
       </c>
       <c r="AB229">
         <v>55322</v>
@@ -57516,12 +57516,12 @@
       </c>
       <c r="AH229" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AI229" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AJ229" t="inlineStr">
@@ -57531,12 +57531,12 @@
       </c>
       <c r="AK229" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AL229" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AM229" t="inlineStr">
@@ -57545,34 +57545,34 @@
         </is>
       </c>
       <c r="AN229">
-        <v>53.5</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="AO229">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="AP229">
-        <v>46.4</v>
+        <v>69.5</v>
       </c>
       <c r="AQ229">
-        <v>42.3</v>
+        <v>28.3</v>
       </c>
       <c r="AR229">
-        <v>53.8</v>
+        <v>100</v>
       </c>
       <c r="AS229">
-        <v>39.4</v>
+        <v>0</v>
       </c>
       <c r="AT229">
-        <v>54</v>
+        <v>75.8</v>
       </c>
       <c r="AU229">
-        <v>42.4</v>
+        <v>24.1</v>
       </c>
       <c r="AV229">
-        <v>50.1</v>
+        <v>72.5</v>
       </c>
       <c r="AW229">
-        <v>46.8</v>
+        <v>27</v>
       </c>
       <c r="AX229" t="inlineStr">
         <is>
@@ -57605,25 +57605,25 @@
         </is>
       </c>
       <c r="BD229">
-        <v>15.74</v>
+        <v>27.84</v>
       </c>
       <c r="BE229" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BF229" t="inlineStr">
         <is>
-          <t>40th percentile</t>
+          <t>60th percentile</t>
         </is>
       </c>
       <c r="BG229" t="inlineStr">
         <is>
-          <t>$33,224.25</t>
+          <t>$32,939.86</t>
         </is>
       </c>
       <c r="BH229">
-        <v>33224.25</v>
+        <v>32939.86</v>
       </c>
       <c r="BI229">
         <v>38182.45</v>
@@ -57642,7 +57642,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -57652,17 +57652,17 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>S001185</t>
+          <t>S001208</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Terri</t>
+          <t>Elissa</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>Sewell</t>
+          <t>Slotkin</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -57672,27 +57672,27 @@
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>MI</t>
         </is>
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>0107</t>
+          <t>2608</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t>H0AL07086</t>
+          <t>H8MI08102</t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="M230" t="inlineStr">
@@ -57701,10 +57701,10 @@
         </is>
       </c>
       <c r="N230">
-        <v>100</v>
+        <v>50.6</v>
       </c>
       <c r="O230">
-        <v>0</v>
+        <v>46.8</v>
       </c>
       <c r="P230" t="inlineStr">
         <is>
@@ -57712,38 +57712,43 @@
         </is>
       </c>
       <c r="Q230">
-        <v>100</v>
+        <v>3.8</v>
       </c>
       <c r="R230" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="S230" t="inlineStr">
         <is>
-          <t>AL-07</t>
+          <t>MI-08</t>
+        </is>
+      </c>
+      <c r="T230" t="inlineStr">
+        <is>
+          <t>tossup</t>
         </is>
       </c>
       <c r="U230">
-        <v>675230</v>
+        <v>723429</v>
       </c>
       <c r="V230">
-        <v>33366</v>
+        <v>65205</v>
       </c>
       <c r="W230">
-        <v>35.8</v>
+        <v>38.1</v>
       </c>
       <c r="X230">
-        <v>2.556</v>
+        <v>7.381</v>
       </c>
       <c r="Y230">
-        <v>7.464</v>
+        <v>6.921</v>
       </c>
       <c r="Z230">
-        <v>67.965</v>
+        <v>17.401</v>
       </c>
       <c r="AA230">
-        <v>19.1</v>
+        <v>39.415</v>
       </c>
       <c r="AB230">
         <v>55322</v>
@@ -57765,12 +57770,12 @@
       </c>
       <c r="AH230" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AI230" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AJ230" t="inlineStr">
@@ -57785,76 +57790,76 @@
       </c>
       <c r="AL230" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AM230" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AN230">
-        <v>98.40000000000001</v>
+        <v>39.2</v>
       </c>
       <c r="AO230">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="AP230">
-        <v>69.5</v>
+        <v>43.8</v>
       </c>
       <c r="AQ230">
-        <v>28.3</v>
+        <v>50.5</v>
       </c>
       <c r="AR230">
-        <v>100</v>
+        <v>42.1</v>
       </c>
       <c r="AS230">
-        <v>0</v>
+        <v>54.6</v>
       </c>
       <c r="AT230">
-        <v>75.8</v>
+        <v>37.3</v>
       </c>
       <c r="AU230">
-        <v>24.1</v>
+        <v>58.6</v>
       </c>
       <c r="AV230">
-        <v>72.5</v>
+        <v>47.9</v>
       </c>
       <c r="AW230">
-        <v>27</v>
+        <v>51.1</v>
       </c>
       <c r="AX230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AY230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AZ230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BA230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BB230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BC230" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BD230">
-        <v>27.84</v>
+        <v>20.77</v>
       </c>
       <c r="BE230" t="inlineStr">
         <is>
@@ -57863,35 +57868,41 @@
       </c>
       <c r="BF230" t="inlineStr">
         <is>
-          <t>60th percentile</t>
+          <t>40th percentile</t>
         </is>
       </c>
       <c r="BG230" t="inlineStr">
         <is>
-          <t>$32,939.86</t>
+          <t>$38,613.36</t>
         </is>
       </c>
       <c r="BH230">
-        <v>32939.86</v>
+        <v>38613.36</v>
       </c>
       <c r="BI230">
         <v>38182.45</v>
       </c>
       <c r="BJ230" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BK230" t="inlineStr">
         <is>
-          <t>NA__D</t>
-        </is>
+          <t>tossup__R</t>
+        </is>
+      </c>
+      <c r="BL230">
+        <v>-16.8</v>
+      </c>
+      <c r="BM230">
+        <v>20.6</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -57901,17 +57912,17 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>S001208</t>
+          <t>T000460</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Elissa</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>Slotkin</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -57921,27 +57932,27 @@
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>MI</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>2608</t>
+          <t>0605</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
         <is>
-          <t>H8MI08102</t>
+          <t>H8CA01109</t>
         </is>
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="M231" t="inlineStr">
@@ -57950,10 +57961,10 @@
         </is>
       </c>
       <c r="N231">
-        <v>50.6</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="O231">
-        <v>46.8</v>
+        <v>0</v>
       </c>
       <c r="P231" t="inlineStr">
         <is>
@@ -57961,43 +57972,38 @@
         </is>
       </c>
       <c r="Q231">
-        <v>3.8</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="R231" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>California</t>
         </is>
       </c>
       <c r="S231" t="inlineStr">
         <is>
-          <t>MI-08</t>
-        </is>
-      </c>
-      <c r="T231" t="inlineStr">
-        <is>
-          <t>tossup</t>
+          <t>CA-05</t>
         </is>
       </c>
       <c r="U231">
-        <v>723429</v>
+        <v>724966</v>
       </c>
       <c r="V231">
-        <v>65205</v>
+        <v>67273</v>
       </c>
       <c r="W231">
-        <v>38.1</v>
+        <v>39.9</v>
       </c>
       <c r="X231">
-        <v>7.381</v>
+        <v>20.832</v>
       </c>
       <c r="Y231">
-        <v>6.921</v>
+        <v>7.423</v>
       </c>
       <c r="Z231">
-        <v>17.401</v>
+        <v>49.417</v>
       </c>
       <c r="AA231">
-        <v>39.415</v>
+        <v>30.383</v>
       </c>
       <c r="AB231">
         <v>55322</v>
@@ -58029,7 +58035,7 @@
       </c>
       <c r="AJ231" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AK231" t="inlineStr">
@@ -58039,7 +58045,7 @@
       </c>
       <c r="AL231" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AM231" t="inlineStr">
@@ -58048,71 +58054,71 @@
         </is>
       </c>
       <c r="AN231">
-        <v>39.2</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="AO231">
-        <v>56</v>
+        <v>23.1</v>
       </c>
       <c r="AP231">
-        <v>43.8</v>
+        <v>68.8</v>
       </c>
       <c r="AQ231">
-        <v>50.5</v>
+        <v>24.2</v>
       </c>
       <c r="AR231">
-        <v>42.1</v>
+        <v>75.7</v>
       </c>
       <c r="AS231">
-        <v>54.6</v>
+        <v>0</v>
       </c>
       <c r="AT231">
-        <v>37.3</v>
+        <v>74.5</v>
       </c>
       <c r="AU231">
-        <v>58.6</v>
+        <v>25.5</v>
       </c>
       <c r="AV231">
-        <v>47.9</v>
+        <v>69.7</v>
       </c>
       <c r="AW231">
-        <v>51.1</v>
+        <v>27.4</v>
       </c>
       <c r="AX231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AY231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AZ231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BA231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BB231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BC231" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BD231">
-        <v>20.77</v>
+        <v>7.79</v>
       </c>
       <c r="BE231" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BF231" t="inlineStr">
@@ -58122,36 +58128,36 @@
       </c>
       <c r="BG231" t="inlineStr">
         <is>
-          <t>$38,613.36</t>
+          <t>$38,160.38</t>
         </is>
       </c>
       <c r="BH231">
-        <v>38613.36</v>
+        <v>38160.38000000001</v>
       </c>
       <c r="BI231">
         <v>38182.45</v>
       </c>
       <c r="BJ231" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BK231" t="inlineStr">
         <is>
-          <t>tossup__R</t>
+          <t>NA__D</t>
         </is>
       </c>
       <c r="BL231">
-        <v>-16.8</v>
+        <v>53.8</v>
       </c>
       <c r="BM231">
-        <v>20.6</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -58161,17 +58167,17 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>T000460</t>
+          <t>T000484</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Xochitl</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Torres Small</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -58181,27 +58187,27 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>0605</t>
+          <t>3502</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
         <is>
-          <t>H8CA01109</t>
+          <t>H8NM02248</t>
         </is>
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="M232" t="inlineStr">
@@ -58210,10 +58216,10 @@
         </is>
       </c>
       <c r="N232">
-        <v>78.90000000000001</v>
+        <v>50.9</v>
       </c>
       <c r="O232">
-        <v>0</v>
+        <v>49.1</v>
       </c>
       <c r="P232" t="inlineStr">
         <is>
@@ -58221,38 +58227,43 @@
         </is>
       </c>
       <c r="Q232">
-        <v>78.90000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="R232" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="S232" t="inlineStr">
         <is>
-          <t>CA-05</t>
+          <t>NM-02</t>
+        </is>
+      </c>
+      <c r="T232" t="inlineStr">
+        <is>
+          <t>tossup</t>
         </is>
       </c>
       <c r="U232">
-        <v>724966</v>
+        <v>698524</v>
       </c>
       <c r="V232">
-        <v>67273</v>
+        <v>41600</v>
       </c>
       <c r="W232">
-        <v>39.9</v>
+        <v>35.9</v>
       </c>
       <c r="X232">
-        <v>20.832</v>
+        <v>11.782</v>
       </c>
       <c r="Y232">
-        <v>7.423</v>
+        <v>10.399</v>
       </c>
       <c r="Z232">
-        <v>49.417</v>
+        <v>62.273</v>
       </c>
       <c r="AA232">
-        <v>30.383</v>
+        <v>20.589</v>
       </c>
       <c r="AB232">
         <v>55322</v>
@@ -58274,22 +58285,22 @@
       </c>
       <c r="AH232" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AI232" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AJ232" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AK232" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AL232" t="inlineStr">
@@ -58299,89 +58310,89 @@
       </c>
       <c r="AM232" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AN232">
-        <v>76.90000000000001</v>
+        <v>37.2</v>
       </c>
       <c r="AO232">
-        <v>23.1</v>
+        <v>62.7</v>
       </c>
       <c r="AP232">
-        <v>68.8</v>
+        <v>39.9</v>
       </c>
       <c r="AQ232">
-        <v>24.2</v>
+        <v>50.1</v>
       </c>
       <c r="AR232">
-        <v>75.7</v>
+        <v>35.5</v>
       </c>
       <c r="AS232">
-        <v>0</v>
+        <v>64.5</v>
       </c>
       <c r="AT232">
-        <v>74.5</v>
+        <v>40.9</v>
       </c>
       <c r="AU232">
-        <v>25.5</v>
+        <v>59.1</v>
       </c>
       <c r="AV232">
-        <v>69.7</v>
+        <v>44.9</v>
       </c>
       <c r="AW232">
-        <v>27.4</v>
+        <v>51.7</v>
       </c>
       <c r="AX232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AY232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AZ232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BA232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BB232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BC232" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BD232">
-        <v>7.79</v>
+        <v>27.96</v>
       </c>
       <c r="BE232" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BF232" t="inlineStr">
         <is>
-          <t>40th percentile</t>
+          <t>60th percentile</t>
         </is>
       </c>
       <c r="BG232" t="inlineStr">
         <is>
-          <t>$38,160.38</t>
+          <t>$24,936.05</t>
         </is>
       </c>
       <c r="BH232">
-        <v>38160.38000000001</v>
+        <v>24936.05</v>
       </c>
       <c r="BI232">
         <v>38182.45</v>
@@ -58393,20 +58404,20 @@
       </c>
       <c r="BK232" t="inlineStr">
         <is>
-          <t>NA__D</t>
+          <t>tossup__R</t>
         </is>
       </c>
       <c r="BL232">
-        <v>53.8</v>
+        <v>-25.5</v>
       </c>
       <c r="BM232">
-        <v>25.1</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -58416,17 +58427,17 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>T000484</t>
+          <t>U000040</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Xochitl</t>
+          <t>Lauren</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>Torres Small</t>
+          <t>Underwood</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
@@ -58436,22 +58447,22 @@
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>3502</t>
+          <t>1714</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
         <is>
-          <t>H8NM02248</t>
+          <t>H8IL14174</t>
         </is>
       </c>
       <c r="L233" t="inlineStr">
@@ -58465,10 +58476,10 @@
         </is>
       </c>
       <c r="N233">
-        <v>50.9</v>
+        <v>52.5</v>
       </c>
       <c r="O233">
-        <v>49.1</v>
+        <v>47.5</v>
       </c>
       <c r="P233" t="inlineStr">
         <is>
@@ -58476,43 +58487,43 @@
         </is>
       </c>
       <c r="Q233">
-        <v>1.8</v>
+        <v>5</v>
       </c>
       <c r="R233" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="S233" t="inlineStr">
         <is>
-          <t>NM-02</t>
+          <t>IL-14</t>
         </is>
       </c>
       <c r="T233" t="inlineStr">
         <is>
-          <t>tossup</t>
+          <t>lean republican</t>
         </is>
       </c>
       <c r="U233">
-        <v>698524</v>
+        <v>725478</v>
       </c>
       <c r="V233">
-        <v>41600</v>
+        <v>86449</v>
       </c>
       <c r="W233">
-        <v>35.9</v>
+        <v>38.8</v>
       </c>
       <c r="X233">
-        <v>11.782</v>
+        <v>9.355</v>
       </c>
       <c r="Y233">
-        <v>10.399</v>
+        <v>6.597</v>
       </c>
       <c r="Z233">
-        <v>62.273</v>
+        <v>20.733</v>
       </c>
       <c r="AA233">
-        <v>20.589</v>
+        <v>39.604</v>
       </c>
       <c r="AB233">
         <v>55322</v>
@@ -58534,12 +58545,12 @@
       </c>
       <c r="AH233" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AI233" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AJ233" t="inlineStr">
@@ -58549,48 +58560,48 @@
       </c>
       <c r="AK233" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AL233" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AM233" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AN233">
-        <v>37.2</v>
+        <v>40.7</v>
       </c>
       <c r="AO233">
-        <v>62.7</v>
+        <v>59.3</v>
       </c>
       <c r="AP233">
-        <v>39.9</v>
+        <v>45.3</v>
       </c>
       <c r="AQ233">
-        <v>50.1</v>
+        <v>49.3</v>
       </c>
       <c r="AR233">
-        <v>35.5</v>
+        <v>34.6</v>
       </c>
       <c r="AS233">
-        <v>64.5</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="AT233">
-        <v>40.9</v>
+        <v>41.2</v>
       </c>
       <c r="AU233">
-        <v>59.1</v>
+        <v>58.8</v>
       </c>
       <c r="AV233">
-        <v>44.9</v>
+        <v>44.2</v>
       </c>
       <c r="AW233">
-        <v>51.7</v>
+        <v>54.2</v>
       </c>
       <c r="AX233" t="inlineStr">
         <is>
@@ -58623,25 +58634,25 @@
         </is>
       </c>
       <c r="BD233">
-        <v>27.96</v>
+        <v>10.14</v>
       </c>
       <c r="BE233" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BF233" t="inlineStr">
         <is>
-          <t>60th percentile</t>
+          <t>40th percentile</t>
         </is>
       </c>
       <c r="BG233" t="inlineStr">
         <is>
-          <t>$24,936.05</t>
+          <t>$30,894.12</t>
         </is>
       </c>
       <c r="BH233">
-        <v>24936.05</v>
+        <v>30894.12</v>
       </c>
       <c r="BI233">
         <v>38182.45</v>
@@ -58653,20 +58664,20 @@
       </c>
       <c r="BK233" t="inlineStr">
         <is>
-          <t>tossup__R</t>
+          <t>lean republican__R</t>
         </is>
       </c>
       <c r="BL233">
-        <v>-25.5</v>
+        <v>-18.59999999999999</v>
       </c>
       <c r="BM233">
-        <v>27.3</v>
+        <v>23.59999999999999</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -58676,17 +58687,17 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>U000040</t>
+          <t>V000133</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Lauren</t>
+          <t>Jefferson</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>Underwood</t>
+          <t>Van Drew</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -58696,22 +58707,22 @@
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>3402</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>H8IL14174</t>
+          <t>H8NJ02166</t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
@@ -58725,10 +58736,10 @@
         </is>
       </c>
       <c r="N234">
-        <v>52.5</v>
+        <v>52.9</v>
       </c>
       <c r="O234">
-        <v>47.5</v>
+        <v>45.2</v>
       </c>
       <c r="P234" t="inlineStr">
         <is>
@@ -58736,43 +58747,43 @@
         </is>
       </c>
       <c r="Q234">
-        <v>5</v>
+        <v>7.7</v>
       </c>
       <c r="R234" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="S234" t="inlineStr">
         <is>
-          <t>IL-14</t>
+          <t>NJ-02</t>
         </is>
       </c>
       <c r="T234" t="inlineStr">
         <is>
-          <t>lean republican</t>
+          <t>likely democratic</t>
         </is>
       </c>
       <c r="U234">
-        <v>725478</v>
+        <v>729824</v>
       </c>
       <c r="V234">
-        <v>86449</v>
+        <v>59785</v>
       </c>
       <c r="W234">
-        <v>38.8</v>
+        <v>41.4</v>
       </c>
       <c r="X234">
-        <v>9.355</v>
+        <v>10.513</v>
       </c>
       <c r="Y234">
-        <v>6.597</v>
+        <v>7.673</v>
       </c>
       <c r="Z234">
-        <v>20.733</v>
+        <v>33.95399999999999</v>
       </c>
       <c r="AA234">
-        <v>39.604</v>
+        <v>24.78</v>
       </c>
       <c r="AB234">
         <v>55322</v>
@@ -58819,38 +58830,38 @@
       </c>
       <c r="AM234" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AN234">
-        <v>40.7</v>
+        <v>37.2</v>
       </c>
       <c r="AO234">
-        <v>59.3</v>
+        <v>59.2</v>
       </c>
       <c r="AP234">
-        <v>45.3</v>
+        <v>46</v>
       </c>
       <c r="AQ234">
-        <v>49.3</v>
+        <v>50.6</v>
       </c>
       <c r="AR234">
-        <v>34.6</v>
+        <v>37.3</v>
       </c>
       <c r="AS234">
-        <v>65.40000000000001</v>
+        <v>61.5</v>
       </c>
       <c r="AT234">
-        <v>41.2</v>
+        <v>40.3</v>
       </c>
       <c r="AU234">
-        <v>58.8</v>
+        <v>57.7</v>
       </c>
       <c r="AV234">
-        <v>44.2</v>
+        <v>53.7</v>
       </c>
       <c r="AW234">
-        <v>54.2</v>
+        <v>45.5</v>
       </c>
       <c r="AX234" t="inlineStr">
         <is>
@@ -58874,16 +58885,16 @@
       </c>
       <c r="BB234" t="inlineStr">
         <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="BC234" t="inlineStr">
+        <is>
           <t>R</t>
         </is>
       </c>
-      <c r="BC234" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
       <c r="BD234">
-        <v>10.14</v>
+        <v>19.45</v>
       </c>
       <c r="BE234" t="inlineStr">
         <is>
@@ -58897,11 +58908,11 @@
       </c>
       <c r="BG234" t="inlineStr">
         <is>
-          <t>$30,894.12</t>
+          <t>$29,925.96</t>
         </is>
       </c>
       <c r="BH234">
-        <v>30894.12</v>
+        <v>29925.96</v>
       </c>
       <c r="BI234">
         <v>38182.45</v>
@@ -58913,20 +58924,20 @@
       </c>
       <c r="BK234" t="inlineStr">
         <is>
-          <t>lean republican__R</t>
+          <t>likely democratic__R</t>
         </is>
       </c>
       <c r="BL234">
-        <v>-18.59999999999999</v>
+        <v>-22</v>
       </c>
       <c r="BM234">
-        <v>23.59999999999999</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>not sponsoring</t>
+          <t>not_sponsoring</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -58936,17 +58947,17 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>V000133</t>
+          <t>V000132</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Jefferson</t>
+          <t>Filemon</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Van Drew</t>
+          <t>Vela</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -58956,27 +58967,27 @@
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>34</t>
         </is>
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>3402</t>
+          <t>4834</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
         <is>
-          <t>H8NJ02166</t>
+          <t>H2TX27190</t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="M235" t="inlineStr">
@@ -58985,10 +58996,10 @@
         </is>
       </c>
       <c r="N235">
-        <v>52.9</v>
+        <v>60</v>
       </c>
       <c r="O235">
-        <v>45.2</v>
+        <v>40</v>
       </c>
       <c r="P235" t="inlineStr">
         <is>
@@ -58996,43 +59007,38 @@
         </is>
       </c>
       <c r="Q235">
-        <v>7.7</v>
+        <v>20</v>
       </c>
       <c r="R235" t="inlineStr">
         <is>
-          <t>New Jersey</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="S235" t="inlineStr">
         <is>
-          <t>NJ-02</t>
-        </is>
-      </c>
-      <c r="T235" t="inlineStr">
-        <is>
-          <t>likely democratic</t>
+          <t>TX-34</t>
         </is>
       </c>
       <c r="U235">
-        <v>729824</v>
+        <v>718321</v>
       </c>
       <c r="V235">
-        <v>59785</v>
+        <v>36417</v>
       </c>
       <c r="W235">
-        <v>41.4</v>
+        <v>32.2</v>
       </c>
       <c r="X235">
-        <v>10.513</v>
+        <v>19.958</v>
       </c>
       <c r="Y235">
-        <v>7.673</v>
+        <v>5.846</v>
       </c>
       <c r="Z235">
-        <v>33.95399999999999</v>
+        <v>85.881</v>
       </c>
       <c r="AA235">
-        <v>24.78</v>
+        <v>15.065</v>
       </c>
       <c r="AB235">
         <v>55322</v>
@@ -59054,17 +59060,17 @@
       </c>
       <c r="AH235" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AI235" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AJ235" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AK235" t="inlineStr">
@@ -59074,7 +59080,7 @@
       </c>
       <c r="AL235" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AM235" t="inlineStr">
@@ -59083,53 +59089,53 @@
         </is>
       </c>
       <c r="AN235">
-        <v>37.2</v>
+        <v>62.7</v>
       </c>
       <c r="AO235">
-        <v>59.2</v>
+        <v>37.3</v>
       </c>
       <c r="AP235">
-        <v>46</v>
+        <v>59.1</v>
       </c>
       <c r="AQ235">
-        <v>50.6</v>
+        <v>37.6</v>
       </c>
       <c r="AR235">
-        <v>37.3</v>
+        <v>59.5</v>
       </c>
       <c r="AS235">
-        <v>61.5</v>
+        <v>38.6</v>
       </c>
       <c r="AT235">
-        <v>40.3</v>
+        <v>61.9</v>
       </c>
       <c r="AU235">
-        <v>57.7</v>
+        <v>36.2</v>
       </c>
       <c r="AV235">
-        <v>53.7</v>
+        <v>60.7</v>
       </c>
       <c r="AW235">
-        <v>45.5</v>
+        <v>38.3</v>
       </c>
       <c r="AX235" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AY235" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AZ235" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BA235" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BB235" t="inlineStr">
@@ -59139,11 +59145,11 @@
       </c>
       <c r="BC235" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BD235">
-        <v>19.45</v>
+        <v>16.04</v>
       </c>
       <c r="BE235" t="inlineStr">
         <is>
@@ -59157,11 +59163,11 @@
       </c>
       <c r="BG235" t="inlineStr">
         <is>
-          <t>$29,925.96</t>
+          <t>$18,865.00</t>
         </is>
       </c>
       <c r="BH235">
-        <v>29925.96</v>
+        <v>18865</v>
       </c>
       <c r="BI235">
         <v>38182.45</v>
@@ -59172,261 +59178,6 @@
         </is>
       </c>
       <c r="BK235" t="inlineStr">
-        <is>
-          <t>likely democratic__R</t>
-        </is>
-      </c>
-      <c r="BL235">
-        <v>-22</v>
-      </c>
-      <c r="BM235">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>not sponsoring</t>
-        </is>
-      </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>not sponsor</t>
-        </is>
-      </c>
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>V000132</t>
-        </is>
-      </c>
-      <c r="D236" t="inlineStr">
-        <is>
-          <t>Filemon</t>
-        </is>
-      </c>
-      <c r="F236" t="inlineStr">
-        <is>
-          <t>Vela</t>
-        </is>
-      </c>
-      <c r="G236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="H236" t="inlineStr">
-        <is>
-          <t>TX</t>
-        </is>
-      </c>
-      <c r="I236" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="J236" t="inlineStr">
-        <is>
-          <t>4834</t>
-        </is>
-      </c>
-      <c r="K236" t="inlineStr">
-        <is>
-          <t>H2TX27190</t>
-        </is>
-      </c>
-      <c r="L236" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="M236" t="inlineStr">
-        <is>
-          <t>called</t>
-        </is>
-      </c>
-      <c r="N236">
-        <v>60</v>
-      </c>
-      <c r="O236">
-        <v>40</v>
-      </c>
-      <c r="P236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="Q236">
-        <v>20</v>
-      </c>
-      <c r="R236" t="inlineStr">
-        <is>
-          <t>Texas</t>
-        </is>
-      </c>
-      <c r="S236" t="inlineStr">
-        <is>
-          <t>TX-34</t>
-        </is>
-      </c>
-      <c r="U236">
-        <v>718321</v>
-      </c>
-      <c r="V236">
-        <v>36417</v>
-      </c>
-      <c r="W236">
-        <v>32.2</v>
-      </c>
-      <c r="X236">
-        <v>19.958</v>
-      </c>
-      <c r="Y236">
-        <v>5.846</v>
-      </c>
-      <c r="Z236">
-        <v>85.881</v>
-      </c>
-      <c r="AA236">
-        <v>15.065</v>
-      </c>
-      <c r="AB236">
-        <v>55322</v>
-      </c>
-      <c r="AC236">
-        <v>37.7</v>
-      </c>
-      <c r="AD236">
-        <v>13.245</v>
-      </c>
-      <c r="AE236">
-        <v>8.007999999999999</v>
-      </c>
-      <c r="AF236">
-        <v>38.045</v>
-      </c>
-      <c r="AG236">
-        <v>30.315</v>
-      </c>
-      <c r="AH236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AI236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AJ236" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="AK236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AL236" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="AM236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AN236">
-        <v>62.7</v>
-      </c>
-      <c r="AO236">
-        <v>37.3</v>
-      </c>
-      <c r="AP236">
-        <v>59.1</v>
-      </c>
-      <c r="AQ236">
-        <v>37.6</v>
-      </c>
-      <c r="AR236">
-        <v>59.5</v>
-      </c>
-      <c r="AS236">
-        <v>38.6</v>
-      </c>
-      <c r="AT236">
-        <v>61.9</v>
-      </c>
-      <c r="AU236">
-        <v>36.2</v>
-      </c>
-      <c r="AV236">
-        <v>60.7</v>
-      </c>
-      <c r="AW236">
-        <v>38.3</v>
-      </c>
-      <c r="AX236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AY236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AZ236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="BA236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="BB236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="BC236" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="BD236">
-        <v>16.04</v>
-      </c>
-      <c r="BE236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="BF236" t="inlineStr">
-        <is>
-          <t>40th percentile</t>
-        </is>
-      </c>
-      <c r="BG236" t="inlineStr">
-        <is>
-          <t>$18,865.00</t>
-        </is>
-      </c>
-      <c r="BH236">
-        <v>18865</v>
-      </c>
-      <c r="BI236">
-        <v>38182.45</v>
-      </c>
-      <c r="BJ236" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="BK236" t="inlineStr">
         <is>
           <t>NA__D</t>
         </is>

</xml_diff>

<commit_message>
add groupings to export as list to multiple xlsx tabs
</commit_message>
<xml_diff>
--- a/output/working_joined_hr1296.xlsx
+++ b/output/working_joined_hr1296.xlsx
@@ -26759,12 +26759,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>L000551</t>
+          <t>L000590</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Susie</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -26779,22 +26779,22 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NV</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>0613</t>
+          <t>3203</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>H8CA09060</t>
+          <t>H8NV03200</t>
         </is>
       </c>
       <c r="L107" t="inlineStr">
@@ -26808,10 +26808,10 @@
         </is>
       </c>
       <c r="N107">
-        <v>88.40000000000001</v>
+        <v>51.9</v>
       </c>
       <c r="O107">
-        <v>0</v>
+        <v>42.8</v>
       </c>
       <c r="P107" t="inlineStr">
         <is>
@@ -26819,38 +26819,43 @@
         </is>
       </c>
       <c r="Q107">
-        <v>88.40000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="S107" t="inlineStr">
         <is>
-          <t>CA-13</t>
+          <t>NV-03</t>
+        </is>
+      </c>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>lean democratic</t>
         </is>
       </c>
       <c r="U107">
-        <v>740683</v>
+        <v>739847</v>
       </c>
       <c r="V107">
-        <v>64948</v>
+        <v>64740</v>
       </c>
       <c r="W107">
-        <v>36.6</v>
+        <v>38.6</v>
       </c>
       <c r="X107">
-        <v>27.069</v>
+        <v>18.367</v>
       </c>
       <c r="Y107">
-        <v>4.351</v>
+        <v>9.875999999999999</v>
       </c>
       <c r="Z107">
-        <v>65.55500000000001</v>
+        <v>42.516</v>
       </c>
       <c r="AA107">
-        <v>46.129</v>
+        <v>31.415</v>
       </c>
       <c r="AB107">
         <v>55322</v>
@@ -26877,7 +26882,7 @@
       </c>
       <c r="AI107" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AJ107" t="inlineStr">
@@ -26887,7 +26892,7 @@
       </c>
       <c r="AK107" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AL107" t="inlineStr">
@@ -26901,34 +26906,34 @@
         </is>
       </c>
       <c r="AN107">
-        <v>90.8</v>
+        <v>47.2</v>
       </c>
       <c r="AO107">
-        <v>9.199999999999999</v>
+        <v>46</v>
       </c>
       <c r="AP107">
-        <v>86</v>
+        <v>46.5</v>
       </c>
       <c r="AQ107">
-        <v>6.7</v>
+        <v>47.5</v>
       </c>
       <c r="AR107">
-        <v>88.5</v>
+        <v>36.1</v>
       </c>
       <c r="AS107">
-        <v>11.5</v>
+        <v>60.8</v>
       </c>
       <c r="AT107">
-        <v>86.8</v>
+        <v>42.9</v>
       </c>
       <c r="AU107">
-        <v>0</v>
+        <v>50.4</v>
       </c>
       <c r="AV107">
-        <v>87.5</v>
+        <v>49.3</v>
       </c>
       <c r="AW107">
-        <v>9</v>
+        <v>48.5</v>
       </c>
       <c r="AX107" t="inlineStr">
         <is>
@@ -26937,17 +26942,17 @@
       </c>
       <c r="AY107" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AZ107" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BA107" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BB107" t="inlineStr">
@@ -26961,7 +26966,7 @@
         </is>
       </c>
       <c r="BD107">
-        <v>0.01</v>
+        <v>1.67</v>
       </c>
       <c r="BE107" t="inlineStr">
         <is>
@@ -26970,28 +26975,28 @@
       </c>
       <c r="BF107" t="inlineStr">
         <is>
-          <t>below 20th percentile</t>
+          <t>20th percentile</t>
         </is>
       </c>
       <c r="BG107" t="inlineStr">
         <is>
-          <t>$53,717.31</t>
+          <t>$33,477.14</t>
         </is>
       </c>
       <c r="BH107">
-        <v>53717.31000000001</v>
+        <v>33477.14</v>
       </c>
       <c r="BI107">
         <v>38182.45</v>
       </c>
       <c r="BJ107" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BK107" t="inlineStr">
         <is>
-          <t>NA__D</t>
+          <t>lean democratic__D</t>
         </is>
       </c>
     </row>
@@ -27008,12 +27013,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>L000590</t>
+          <t>L000551</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Susie</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -27028,22 +27033,22 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>3203</t>
+          <t>0613</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>H8NV03200</t>
+          <t>H8CA09060</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
@@ -27057,10 +27062,10 @@
         </is>
       </c>
       <c r="N108">
-        <v>51.9</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="O108">
-        <v>42.8</v>
+        <v>0</v>
       </c>
       <c r="P108" t="inlineStr">
         <is>
@@ -27068,43 +27073,38 @@
         </is>
       </c>
       <c r="Q108">
-        <v>9.1</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>California</t>
         </is>
       </c>
       <c r="S108" t="inlineStr">
         <is>
-          <t>NV-03</t>
-        </is>
-      </c>
-      <c r="T108" t="inlineStr">
-        <is>
-          <t>lean democratic</t>
+          <t>CA-13</t>
         </is>
       </c>
       <c r="U108">
-        <v>739847</v>
+        <v>740683</v>
       </c>
       <c r="V108">
-        <v>64740</v>
+        <v>64948</v>
       </c>
       <c r="W108">
-        <v>38.6</v>
+        <v>36.6</v>
       </c>
       <c r="X108">
-        <v>18.367</v>
+        <v>27.069</v>
       </c>
       <c r="Y108">
-        <v>9.875999999999999</v>
+        <v>4.351</v>
       </c>
       <c r="Z108">
-        <v>42.516</v>
+        <v>65.55500000000001</v>
       </c>
       <c r="AA108">
-        <v>31.415</v>
+        <v>46.129</v>
       </c>
       <c r="AB108">
         <v>55322</v>
@@ -27131,7 +27131,7 @@
       </c>
       <c r="AI108" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AJ108" t="inlineStr">
@@ -27141,7 +27141,7 @@
       </c>
       <c r="AK108" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AL108" t="inlineStr">
@@ -27155,34 +27155,34 @@
         </is>
       </c>
       <c r="AN108">
-        <v>47.2</v>
+        <v>90.8</v>
       </c>
       <c r="AO108">
-        <v>46</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AP108">
-        <v>46.5</v>
+        <v>86</v>
       </c>
       <c r="AQ108">
-        <v>47.5</v>
+        <v>6.7</v>
       </c>
       <c r="AR108">
-        <v>36.1</v>
+        <v>88.5</v>
       </c>
       <c r="AS108">
-        <v>60.8</v>
+        <v>11.5</v>
       </c>
       <c r="AT108">
-        <v>42.9</v>
+        <v>86.8</v>
       </c>
       <c r="AU108">
-        <v>50.4</v>
+        <v>0</v>
       </c>
       <c r="AV108">
-        <v>49.3</v>
+        <v>87.5</v>
       </c>
       <c r="AW108">
-        <v>48.5</v>
+        <v>9</v>
       </c>
       <c r="AX108" t="inlineStr">
         <is>
@@ -27191,17 +27191,17 @@
       </c>
       <c r="AY108" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AZ108" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BA108" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BB108" t="inlineStr">
@@ -27215,7 +27215,7 @@
         </is>
       </c>
       <c r="BD108">
-        <v>1.67</v>
+        <v>0.01</v>
       </c>
       <c r="BE108" t="inlineStr">
         <is>
@@ -27224,28 +27224,28 @@
       </c>
       <c r="BF108" t="inlineStr">
         <is>
-          <t>20th percentile</t>
+          <t>below 20th percentile</t>
         </is>
       </c>
       <c r="BG108" t="inlineStr">
         <is>
-          <t>$33,477.14</t>
+          <t>$53,717.31</t>
         </is>
       </c>
       <c r="BH108">
-        <v>33477.14</v>
+        <v>53717.31000000001</v>
       </c>
       <c r="BI108">
         <v>38182.45</v>
       </c>
       <c r="BJ108" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BK108" t="inlineStr">
         <is>
-          <t>lean democratic__D</t>
+          <t>NA__D</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add export; updated outputs
</commit_message>
<xml_diff>
--- a/output/working_joined_hr1296.xlsx
+++ b/output/working_joined_hr1296.xlsx
@@ -27289,12 +27289,12 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>L000590</t>
+          <t>L000551</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Susie</t>
+          <t>Barbara</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -27309,22 +27309,22 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>3203</t>
+          <t>0613</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>H8NV03200</t>
+          <t>H8CA09060</t>
         </is>
       </c>
       <c r="L107" t="inlineStr">
@@ -27338,10 +27338,10 @@
         </is>
       </c>
       <c r="N107">
-        <v>51.9</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="O107">
-        <v>42.8</v>
+        <v>0</v>
       </c>
       <c r="P107" t="inlineStr">
         <is>
@@ -27349,43 +27349,38 @@
         </is>
       </c>
       <c r="Q107">
-        <v>9.1</v>
+        <v>88.40000000000001</v>
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>Nevada</t>
+          <t>California</t>
         </is>
       </c>
       <c r="S107" t="inlineStr">
         <is>
-          <t>NV-03</t>
-        </is>
-      </c>
-      <c r="T107" t="inlineStr">
-        <is>
-          <t>lean democratic</t>
+          <t>CA-13</t>
         </is>
       </c>
       <c r="U107">
-        <v>739847</v>
+        <v>740683</v>
       </c>
       <c r="V107">
-        <v>64740</v>
+        <v>64948</v>
       </c>
       <c r="W107">
-        <v>38.6</v>
+        <v>36.6</v>
       </c>
       <c r="X107">
-        <v>18.367</v>
+        <v>27.069</v>
       </c>
       <c r="Y107">
-        <v>9.875999999999999</v>
+        <v>4.351</v>
       </c>
       <c r="Z107">
-        <v>42.516</v>
+        <v>65.55500000000001</v>
       </c>
       <c r="AA107">
-        <v>31.415</v>
+        <v>46.129</v>
       </c>
       <c r="AB107">
         <v>55322</v>
@@ -27412,7 +27407,7 @@
       </c>
       <c r="AI107" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AJ107" t="inlineStr">
@@ -27422,7 +27417,7 @@
       </c>
       <c r="AK107" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AL107" t="inlineStr">
@@ -27436,34 +27431,34 @@
         </is>
       </c>
       <c r="AN107">
-        <v>47.2</v>
+        <v>90.8</v>
       </c>
       <c r="AO107">
-        <v>46</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="AP107">
-        <v>46.5</v>
+        <v>86</v>
       </c>
       <c r="AQ107">
-        <v>47.5</v>
+        <v>6.7</v>
       </c>
       <c r="AR107">
-        <v>36.1</v>
+        <v>88.5</v>
       </c>
       <c r="AS107">
-        <v>60.8</v>
+        <v>11.5</v>
       </c>
       <c r="AT107">
-        <v>42.9</v>
+        <v>86.8</v>
       </c>
       <c r="AU107">
-        <v>50.4</v>
+        <v>0</v>
       </c>
       <c r="AV107">
-        <v>49.3</v>
+        <v>87.5</v>
       </c>
       <c r="AW107">
-        <v>48.5</v>
+        <v>9</v>
       </c>
       <c r="AX107" t="inlineStr">
         <is>
@@ -27472,17 +27467,17 @@
       </c>
       <c r="AY107" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AZ107" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BA107" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="BB107" t="inlineStr">
@@ -27496,7 +27491,7 @@
         </is>
       </c>
       <c r="BD107">
-        <v>1.67</v>
+        <v>0.01</v>
       </c>
       <c r="BE107" t="inlineStr">
         <is>
@@ -27505,28 +27500,28 @@
       </c>
       <c r="BF107" t="inlineStr">
         <is>
-          <t>20th percentile</t>
+          <t>below 20th percentile</t>
         </is>
       </c>
       <c r="BG107" t="inlineStr">
         <is>
-          <t>$33,477.14</t>
+          <t>$53,717.31</t>
         </is>
       </c>
       <c r="BH107">
-        <v>33477.14</v>
+        <v>53717.31000000001</v>
       </c>
       <c r="BI107">
         <v>38182.45</v>
       </c>
       <c r="BJ107" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="BK107" t="inlineStr">
         <is>
-          <t>lean democratic__D</t>
+          <t>NA__D</t>
         </is>
       </c>
       <c r="BN107" t="inlineStr">
@@ -27548,12 +27543,12 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>L000551</t>
+          <t>L000590</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Barbara</t>
+          <t>Susie</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -27568,22 +27563,22 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NV</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>0613</t>
+          <t>3203</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>H8CA09060</t>
+          <t>H8NV03200</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
@@ -27597,10 +27592,10 @@
         </is>
       </c>
       <c r="N108">
-        <v>88.40000000000001</v>
+        <v>51.9</v>
       </c>
       <c r="O108">
-        <v>0</v>
+        <v>42.8</v>
       </c>
       <c r="P108" t="inlineStr">
         <is>
@@ -27608,38 +27603,43 @@
         </is>
       </c>
       <c r="Q108">
-        <v>88.40000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="S108" t="inlineStr">
         <is>
-          <t>CA-13</t>
+          <t>NV-03</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>lean democratic</t>
         </is>
       </c>
       <c r="U108">
-        <v>740683</v>
+        <v>739847</v>
       </c>
       <c r="V108">
-        <v>64948</v>
+        <v>64740</v>
       </c>
       <c r="W108">
-        <v>36.6</v>
+        <v>38.6</v>
       </c>
       <c r="X108">
-        <v>27.069</v>
+        <v>18.367</v>
       </c>
       <c r="Y108">
-        <v>4.351</v>
+        <v>9.875999999999999</v>
       </c>
       <c r="Z108">
-        <v>65.55500000000001</v>
+        <v>42.516</v>
       </c>
       <c r="AA108">
-        <v>46.129</v>
+        <v>31.415</v>
       </c>
       <c r="AB108">
         <v>55322</v>
@@ -27666,7 +27666,7 @@
       </c>
       <c r="AI108" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AJ108" t="inlineStr">
@@ -27676,7 +27676,7 @@
       </c>
       <c r="AK108" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AL108" t="inlineStr">
@@ -27690,34 +27690,34 @@
         </is>
       </c>
       <c r="AN108">
-        <v>90.8</v>
+        <v>47.2</v>
       </c>
       <c r="AO108">
-        <v>9.199999999999999</v>
+        <v>46</v>
       </c>
       <c r="AP108">
-        <v>86</v>
+        <v>46.5</v>
       </c>
       <c r="AQ108">
-        <v>6.7</v>
+        <v>47.5</v>
       </c>
       <c r="AR108">
-        <v>88.5</v>
+        <v>36.1</v>
       </c>
       <c r="AS108">
-        <v>11.5</v>
+        <v>60.8</v>
       </c>
       <c r="AT108">
-        <v>86.8</v>
+        <v>42.9</v>
       </c>
       <c r="AU108">
-        <v>0</v>
+        <v>50.4</v>
       </c>
       <c r="AV108">
-        <v>87.5</v>
+        <v>49.3</v>
       </c>
       <c r="AW108">
-        <v>9</v>
+        <v>48.5</v>
       </c>
       <c r="AX108" t="inlineStr">
         <is>
@@ -27726,17 +27726,17 @@
       </c>
       <c r="AY108" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AZ108" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BA108" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="BB108" t="inlineStr">
@@ -27750,7 +27750,7 @@
         </is>
       </c>
       <c r="BD108">
-        <v>0.01</v>
+        <v>1.67</v>
       </c>
       <c r="BE108" t="inlineStr">
         <is>
@@ -27759,28 +27759,28 @@
       </c>
       <c r="BF108" t="inlineStr">
         <is>
-          <t>below 20th percentile</t>
+          <t>20th percentile</t>
         </is>
       </c>
       <c r="BG108" t="inlineStr">
         <is>
-          <t>$53,717.31</t>
+          <t>$33,477.14</t>
         </is>
       </c>
       <c r="BH108">
-        <v>53717.31000000001</v>
+        <v>33477.14</v>
       </c>
       <c r="BI108">
         <v>38182.45</v>
       </c>
       <c r="BJ108" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="BK108" t="inlineStr">
         <is>
-          <t>NA__D</t>
+          <t>lean democratic__D</t>
         </is>
       </c>
       <c r="BN108" t="inlineStr">

</xml_diff>